<commit_message>
modify sql file and add execute sql bat
</commit_message>
<xml_diff>
--- a/03_プログラム設計書/SQL設計.xlsx
+++ b/03_プログラム設計書/SQL設計.xlsx
@@ -61,10 +61,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>endWorkingTask</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>update</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -76,27 +72,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>registTask</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>getAllTaskContentList</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>getAllTaskNoteList</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>insert</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>registUser</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>getWorkingTask</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -322,24 +302,38 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>deleteTask</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>updataTask</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>insertTask</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>getTaskList</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Users
 User_role</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>getAllWorkContentList</t>
+  </si>
+  <si>
+    <t>getAllWorkNoteList</t>
+  </si>
+  <si>
+    <t>getWorkList</t>
+  </si>
+  <si>
+    <t>insertWork</t>
+  </si>
+  <si>
+    <t>deleteWork</t>
+  </si>
+  <si>
+    <t>updataWork</t>
+  </si>
+  <si>
+    <t>getWorking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>endWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>registWork</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -370,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +374,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -437,6 +437,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -767,31 +773,31 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>46</v>
@@ -805,37 +811,37 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
@@ -843,19 +849,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>5</v>
@@ -867,51 +873,51 @@
         <v>5</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="81" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="94.5" x14ac:dyDescent="0.15">
@@ -919,75 +925,75 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="148.5" x14ac:dyDescent="0.15">
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="K7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="40.5" x14ac:dyDescent="0.15">
@@ -995,37 +1001,37 @@
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
modify sqlfile and sql specification
</commit_message>
<xml_diff>
--- a/03_プログラム設計書/SQL設計.xlsx
+++ b/03_プログラム設計書/SQL設計.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>SQL名</t>
     <rPh sb="3" eb="4">
@@ -92,30 +92,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>①id
-②user_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>id = ①
-ユーザid = ②</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>insert</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>①user_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>note</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ユーザid = ①
-deleteFlg = 0</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -154,21 +135,6 @@
     <t>★jdbcレルムで使用？
 不要かも。</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>①user_id
-②content
-③note</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Users.user_id
-Users.user_name
-Users.password
-User_role.role
-User_role.user_id
-</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>startTime
@@ -179,11 +145,119 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>①user_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>①user_id
+    <t xml:space="preserve">startTime　= ③
+endTime　= ④
+workingTime　= ⑤
+content　= ⑥
+note　= ⑦
+uptime = 現在時間
+</t>
+    <rPh sb="72" eb="74">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>startTime
+content
+note</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>getAllWorkContentList</t>
+  </si>
+  <si>
+    <t>getAllWorkNoteList</t>
+  </si>
+  <si>
+    <t>getWorkList</t>
+  </si>
+  <si>
+    <t>updataWork</t>
+  </si>
+  <si>
+    <t>getWorking</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>endWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>registWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>insertWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>getStartTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>getEndTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>startTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>endTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①id
+②content
+③note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users.id
+Users.user_name
+Users.password
+User_role.role
+User_role.id
+</t>
+  </si>
+  <si>
+    <t>id = 自動インクリメント
+id　= ①
+startTime　= 現在時間
+endTime　= ""
+workingTime　= ""
+content　= ③
+note　= ④
+workdate = 現在年月日
+uptime = 現在時間
+deleteFlg = 0</t>
+    <rPh sb="5" eb="7">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="101" eb="103">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="103" eb="106">
+      <t>ネンガッピ</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="118" eb="120">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①id
+②user_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①id
 ②startTime
 ③endTime
 ④workingTime
@@ -193,7 +267,6 @@
   </si>
   <si>
     <t xml:space="preserve">id = 自動インクリメント
-user_id　= ①
 startTime　= ②
 endTime　= ③
 workingTime　= ④
@@ -206,66 +279,41 @@
     <rPh sb="5" eb="7">
       <t>ジドウ</t>
     </rPh>
-    <rPh sb="101" eb="103">
+    <rPh sb="89" eb="91">
       <t>ゲンザイ</t>
     </rPh>
-    <rPh sb="103" eb="106">
+    <rPh sb="91" eb="94">
       <t>ネンガッピ</t>
     </rPh>
-    <rPh sb="116" eb="118">
+    <rPh sb="104" eb="106">
       <t>ゲンザイ</t>
     </rPh>
-    <rPh sb="118" eb="120">
+    <rPh sb="106" eb="108">
       <t>ジカン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>id = 自動インクリメント
-user_id　= ①
-startTime　= 現在時間
-endTime　= ""
-workingTime　= ""
-content　= ③
-note　= ④
-workdate = 現在年月日
-uptime = 現在時間
+    <t>id = ①
+user_name = ②
+deleteFlg = 0
+endTime &lt;&gt; ""</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id = ①
+user_name = ②
 deleteFlg = 0</t>
-    <rPh sb="5" eb="7">
-      <t>ジドウ</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="108" eb="111">
-      <t>ネンガッピ</t>
-    </rPh>
-    <rPh sb="121" eb="123">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>ジカン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Users.user_id = 自動インクリメント
-Users.user_name = ①
-Users.password = ②
-User_role.role = ③
-User_role.user_id = Users.user_id</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">①Users.user_name
-②Users.password
-③User_role.role
-</t>
-    <phoneticPr fontId="2"/>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id = ①
+user_name = ②</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>①id
-②user_id
+②user_name
 ③startTime
 ④endTime
 ⑤workingTime
@@ -274,66 +322,41 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">startTime　= ③
-endTime　= ④
-workingTime　= ⑤
-content　= ⑥
-note　= ⑦
-uptime = 現在時間
+    <t>registRole</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Users</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①user_name
+②password</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">①user_name
+②role
 </t>
-    <rPh sb="72" eb="74">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>ジカン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>startTime
-content
-note</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ユーザid = ①
-deleteFlg = 0
-endTime &lt;&gt; ""</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Users
-User_role</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>getAllWorkContentList</t>
-  </si>
-  <si>
-    <t>getAllWorkNoteList</t>
-  </si>
-  <si>
-    <t>getWorkList</t>
-  </si>
-  <si>
-    <t>insertWork</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>user_name = ①
+role = ②</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id = 自動インクリメント
+user_name = ①
+password = ②</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>deleteWork</t>
-  </si>
-  <si>
-    <t>updataWork</t>
-  </si>
-  <si>
-    <t>getWorking</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>endWork</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>registWork</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -745,82 +768,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M9"/>
+  <dimension ref="B2:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1.25" customWidth="1"/>
     <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.375" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.75" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.125" customWidth="1"/>
+    <col min="3" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.75" customWidth="1"/>
+    <col min="8" max="8" width="21.875" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.25" customWidth="1"/>
+    <col min="14" max="14" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="27" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:16" ht="27" x14ac:dyDescent="0.15">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -838,33 +871,42 @@
         <v>9</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="N3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>5</v>
@@ -873,173 +915,219 @@
         <v>5</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="81" x14ac:dyDescent="0.15">
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="81" x14ac:dyDescent="0.15">
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>30</v>
+      <c r="J5" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="N5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="2:13" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:16" ht="94.5" x14ac:dyDescent="0.15">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="135" x14ac:dyDescent="0.15">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>37</v>
+      <c r="C7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="148.5" x14ac:dyDescent="0.15">
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:16" ht="54" x14ac:dyDescent="0.15">
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>17</v>
+        <v>46</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.15">
       <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>